<commit_message>
Added bracket and odds
</commit_message>
<xml_diff>
--- a/NFL2019/Weekly Forecasts/WeekConMatrix.xlsx
+++ b/NFL2019/Weekly Forecasts/WeekConMatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MerrerPredictifier\MerrerPredictifier\NFL2019\Weekly Forecasts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E147230-60BA-4C6B-942C-1A4840377099}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8698104C-1F20-4708-A10E-89F9642BBE40}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projected Bracket" sheetId="5" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="46">
   <si>
     <t>Chance of Winning</t>
   </si>
@@ -170,6 +170,18 @@
   </si>
   <si>
     <t>San Francisco</t>
+  </si>
+  <si>
+    <t>3/2</t>
+  </si>
+  <si>
+    <t>2/1</t>
+  </si>
+  <si>
+    <t>6/1</t>
+  </si>
+  <si>
+    <t>11/1</t>
   </si>
 </sst>
 </file>
@@ -619,7 +631,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -661,102 +673,102 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -769,6 +781,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1116,7 +1129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B6138F7-FC74-42BD-AD66-9B8CE0ACCCC6}">
   <dimension ref="B1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
@@ -1155,16 +1168,16 @@
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="16"/>
+      <c r="I3" s="44"/>
       <c r="J3" s="14"/>
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
       <c r="M3" s="14"/>
       <c r="N3" s="14"/>
-      <c r="O3" s="17"/>
+      <c r="O3" s="15"/>
     </row>
     <row r="4" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="13"/>
@@ -1173,16 +1186,16 @@
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="19"/>
+      <c r="I4" s="46"/>
       <c r="J4" s="14"/>
       <c r="K4" s="14"/>
       <c r="L4" s="14"/>
       <c r="M4" s="14"/>
       <c r="N4" s="14"/>
-      <c r="O4" s="17"/>
+      <c r="O4" s="15"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B5" s="13"/>
@@ -1200,7 +1213,7 @@
       <c r="L5" s="14"/>
       <c r="M5" s="14"/>
       <c r="N5" s="14"/>
-      <c r="O5" s="17"/>
+      <c r="O5" s="15"/>
     </row>
     <row r="6" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="13"/>
@@ -1218,7 +1231,7 @@
       <c r="L6" s="14"/>
       <c r="M6" s="14"/>
       <c r="N6" s="14"/>
-      <c r="O6" s="17"/>
+      <c r="O6" s="15"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B7" s="13"/>
@@ -1228,13 +1241,13 @@
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
-      <c r="I7" s="20"/>
+      <c r="I7" s="16"/>
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
       <c r="L7" s="14"/>
       <c r="M7" s="14"/>
       <c r="N7" s="14"/>
-      <c r="O7" s="17"/>
+      <c r="O7" s="15"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B8" s="13"/>
@@ -1254,7 +1267,7 @@
       <c r="L8" s="14"/>
       <c r="M8" s="14"/>
       <c r="N8" s="14"/>
-      <c r="O8" s="17"/>
+      <c r="O8" s="15"/>
     </row>
     <row r="9" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="13"/>
@@ -1262,19 +1275,19 @@
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="45">
+      <c r="G9" s="18"/>
+      <c r="H9" s="41">
         <v>25.411199799999999</v>
       </c>
-      <c r="I9" s="46">
+      <c r="I9" s="42">
         <v>26.279170199999999</v>
       </c>
-      <c r="J9" s="23"/>
-      <c r="K9" s="24"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="20"/>
       <c r="L9" s="14"/>
       <c r="M9" s="14"/>
       <c r="N9" s="14"/>
-      <c r="O9" s="17"/>
+      <c r="O9" s="15"/>
     </row>
     <row r="10" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="13"/>
@@ -1282,15 +1295,15 @@
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
-      <c r="G10" s="24"/>
+      <c r="G10" s="20"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
-      <c r="K10" s="24"/>
+      <c r="K10" s="20"/>
       <c r="L10" s="14"/>
       <c r="M10" s="14"/>
       <c r="N10" s="14"/>
-      <c r="O10" s="17"/>
+      <c r="O10" s="15"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B11" s="13"/>
@@ -1305,216 +1318,216 @@
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
-      <c r="J11" s="26" t="s">
+      <c r="J11" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="K11" s="27" t="s">
+      <c r="K11" s="23" t="s">
         <v>25</v>
       </c>
       <c r="L11" s="14"/>
       <c r="M11" s="14"/>
       <c r="N11" s="14"/>
-      <c r="O11" s="17"/>
+      <c r="O11" s="15"/>
     </row>
     <row r="12" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="13"/>
       <c r="C12" s="14"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="28">
+      <c r="D12" s="18"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="24">
         <v>26.455082999999998</v>
       </c>
-      <c r="G12" s="29">
+      <c r="G12" s="25">
         <v>22.386313600000001</v>
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
-      <c r="J12" s="28">
+      <c r="J12" s="24">
         <v>26.7054598</v>
       </c>
-      <c r="K12" s="29">
+      <c r="K12" s="25">
         <v>19.361739</v>
       </c>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="17"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="15"/>
     </row>
     <row r="13" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="13"/>
       <c r="C13" s="14"/>
-      <c r="D13" s="24"/>
+      <c r="D13" s="20"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
-      <c r="G13" s="24"/>
+      <c r="G13" s="20"/>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
-      <c r="K13" s="24"/>
+      <c r="K13" s="20"/>
       <c r="L13" s="14"/>
       <c r="M13" s="14"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="17"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="15"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B14" s="13"/>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="26" t="s">
         <v>34</v>
       </c>
       <c r="E14" s="14"/>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="27" t="s">
         <v>22</v>
       </c>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
-      <c r="J14" s="26" t="s">
+      <c r="J14" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="K14" s="32" t="s">
+      <c r="K14" s="28" t="s">
         <v>35</v>
       </c>
       <c r="L14" s="14"/>
-      <c r="M14" s="27" t="s">
+      <c r="M14" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="N14" s="33" t="s">
+      <c r="N14" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="O14" s="17"/>
+      <c r="O14" s="15"/>
     </row>
     <row r="15" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="13"/>
-      <c r="C15" s="38">
+      <c r="C15" s="34">
         <v>51</v>
       </c>
-      <c r="D15" s="39">
+      <c r="D15" s="35">
         <v>31</v>
       </c>
       <c r="E15" s="14"/>
-      <c r="F15" s="40">
+      <c r="F15" s="36">
         <v>12</v>
       </c>
-      <c r="G15" s="41">
+      <c r="G15" s="37">
         <v>28</v>
       </c>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
-      <c r="J15" s="38">
+      <c r="J15" s="34">
         <v>27</v>
       </c>
-      <c r="K15" s="39">
+      <c r="K15" s="35">
         <v>10</v>
       </c>
       <c r="L15" s="14"/>
-      <c r="M15" s="38">
+      <c r="M15" s="34">
         <v>28</v>
       </c>
-      <c r="N15" s="39">
+      <c r="N15" s="35">
         <v>23</v>
       </c>
-      <c r="O15" s="17"/>
+      <c r="O15" s="15"/>
     </row>
     <row r="16" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="13"/>
       <c r="C16" s="14"/>
-      <c r="D16" s="24"/>
+      <c r="D16" s="20"/>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
-      <c r="G16" s="24"/>
+      <c r="G16" s="20"/>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
-      <c r="K16" s="24"/>
+      <c r="K16" s="20"/>
       <c r="L16" s="14"/>
       <c r="M16" s="14"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="17"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="15"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B17" s="13"/>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D17" s="30" t="s">
         <v>37</v>
       </c>
       <c r="E17" s="14"/>
-      <c r="F17" s="35" t="s">
+      <c r="F17" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="G17" s="31" t="s">
+      <c r="G17" s="27" t="s">
         <v>22</v>
       </c>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
-      <c r="J17" s="36" t="s">
+      <c r="J17" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="K17" s="32" t="s">
+      <c r="K17" s="28" t="s">
         <v>35</v>
       </c>
       <c r="L17" s="14"/>
-      <c r="M17" s="37" t="s">
+      <c r="M17" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="N17" s="33" t="s">
+      <c r="N17" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="O17" s="17"/>
+      <c r="O17" s="15"/>
     </row>
     <row r="18" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="13"/>
-      <c r="C18" s="38">
+      <c r="C18" s="34">
         <v>22</v>
       </c>
-      <c r="D18" s="39">
+      <c r="D18" s="35">
         <v>19</v>
       </c>
       <c r="E18" s="14"/>
-      <c r="F18" s="40">
+      <c r="F18" s="36">
         <v>13</v>
       </c>
-      <c r="G18" s="41">
+      <c r="G18" s="37">
         <v>20</v>
       </c>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
-      <c r="J18" s="40">
+      <c r="J18" s="36">
         <v>20</v>
       </c>
-      <c r="K18" s="41">
+      <c r="K18" s="37">
         <v>26</v>
       </c>
       <c r="L18" s="14"/>
-      <c r="M18" s="40">
+      <c r="M18" s="36">
         <v>9</v>
       </c>
-      <c r="N18" s="41">
+      <c r="N18" s="37">
         <v>17</v>
       </c>
-      <c r="O18" s="17"/>
+      <c r="O18" s="15"/>
     </row>
     <row r="19" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="42"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="43"/>
-      <c r="N19" s="43"/>
-      <c r="O19" s="44"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1532,8 +1545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E139292C-5B7B-4AF4-AE5D-41CDEEFEB2AF}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1668,6 +1681,13 @@
       <c r="B14" s="9">
         <v>0.43381048844244652</v>
       </c>
+      <c r="C14">
+        <f>ROUND(1/B14-1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="D14" s="51" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -1676,6 +1696,13 @@
       <c r="B15" s="9">
         <v>0.35090436193299696</v>
       </c>
+      <c r="C15">
+        <f>ROUND(1/B15-1, 0)</f>
+        <v>2</v>
+      </c>
+      <c r="D15" s="51" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -1684,13 +1711,27 @@
       <c r="B16" s="9">
         <v>0.13493333537066618</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16">
+        <f>ROUND(1/B16-1, 0)</f>
+        <v>6</v>
+      </c>
+      <c r="D16" s="51" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="9">
         <v>8.0351814253890277E-2</v>
+      </c>
+      <c r="C17">
+        <f>ROUND(1/B17-1, 0)</f>
+        <v>11</v>
+      </c>
+      <c r="D17" s="51" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>